<commit_message>
Sped and new maps
</commit_message>
<xml_diff>
--- a/Enemy-Data.xlsx
+++ b/Enemy-Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Marine</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Elite</t>
+  </si>
+  <si>
+    <t>Spec-Ops</t>
   </si>
 </sst>
 </file>
@@ -257,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -270,6 +273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -553,7 +557,7 @@
   <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,7 +606,7 @@
       </c>
       <c r="F3" s="9"/>
       <c r="H3" s="9">
-        <f t="shared" ref="H3:H11" si="0">C3*((D3*40)/32)</f>
+        <f t="shared" ref="H3:H12" si="0">C3*((D3*40)/32)</f>
         <v>15</v>
       </c>
     </row>
@@ -630,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="8">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D5" s="8">
         <v>0.2</v>
@@ -643,7 +647,7 @@
       </c>
       <c r="H5" s="8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -693,7 +697,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="8">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D8" s="8">
         <v>0.6</v>
@@ -706,7 +710,7 @@
       </c>
       <c r="H8" s="8">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -770,6 +774,27 @@
       <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="12">
+        <v>35</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="0"/>
+        <v>43.75</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
keine Upgrades? gehts noch????
</commit_message>
<xml_diff>
--- a/Enemy-Data.xlsx
+++ b/Enemy-Data.xlsx
@@ -557,7 +557,7 @@
   <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="8">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D4" s="8">
         <v>0.65</v>
@@ -626,7 +626,7 @@
       <c r="F4" s="8"/>
       <c r="H4" s="8">
         <f t="shared" si="0"/>
-        <v>28.4375</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -634,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="8">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D5" s="8">
         <v>0.3</v>
@@ -647,7 +647,7 @@
       </c>
       <c r="H5" s="8">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8">
         <v>1.2</v>
@@ -668,7 +668,7 @@
       </c>
       <c r="H6" s="8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -676,7 +676,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="8">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D7" s="8">
         <v>0.8</v>
@@ -689,7 +689,7 @@
       </c>
       <c r="H7" s="8">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="8">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="D8" s="8">
         <v>0.4</v>
@@ -710,7 +710,7 @@
       </c>
       <c r="H8" s="8">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -718,7 +718,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="8">
         <v>0.6</v>
@@ -731,7 +731,7 @@
       </c>
       <c r="H9" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -739,7 +739,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="8">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8">
         <v>1.2</v>
@@ -752,7 +752,7 @@
       </c>
       <c r="H10" s="8">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -760,7 +760,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="8">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="D11" s="8">
         <v>0.2</v>
@@ -773,15 +773,15 @@
       </c>
       <c r="H11" s="8">
         <f t="shared" si="0"/>
-        <v>62.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="12">
-        <v>35</v>
+      <c r="C12" s="8">
+        <v>30</v>
       </c>
       <c r="D12" s="12">
         <v>0.75</v>
@@ -794,7 +794,7 @@
       </c>
       <c r="H12" s="12">
         <f t="shared" si="0"/>
-        <v>32.8125</v>
+        <v>28.125</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
startguthaben neueWaves und balancing
</commit_message>
<xml_diff>
--- a/Enemy-Data.xlsx
+++ b/Enemy-Data.xlsx
@@ -557,7 +557,7 @@
   <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +718,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="8">
         <v>0.6</v>
@@ -731,7 +731,7 @@
       </c>
       <c r="H9" s="8">
         <f t="shared" si="0"/>
-        <v>13.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -760,10 +760,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="8">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D11" s="8">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E11" s="8">
         <v>1</v>
@@ -773,7 +773,7 @@
       </c>
       <c r="H11" s="8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>